<commit_message>
css ad admin not work
</commit_message>
<xml_diff>
--- a/stuff/Reda Poker Tour.xlsx
+++ b/stuff/Reda Poker Tour.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="136">
   <si>
     <t>NickName</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>2014-12-19</t>
+  </si>
+  <si>
+    <t>2015-01-02</t>
   </si>
 </sst>
 </file>
@@ -1535,11 +1538,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M413"/>
+  <dimension ref="A1:M420"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L393" sqref="L393:L409"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L410" sqref="L410:L420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9033,18 +9036,18 @@
         <v>562.5</v>
       </c>
       <c r="J298">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K298">
         <v>5</v>
       </c>
       <c r="L298" t="str">
-        <f t="shared" ref="L298:L305" si="49">CONCATENATE("{ player_id: """,G298,""", pos: ",H298,", points: ",I298,", money: ",J298,", pay: ",K298,"},")</f>
-        <v>{ player_id: "Tiga", pos: 1, points: 562.5, money: 50, pay: 5},</v>
+        <f t="shared" ref="L298:L306" si="49">CONCATENATE("{ player_id: """,G298,""", pos: ",H298,", points: ",I298,", money: ",J298,", pay: ",K298,"},")</f>
+        <v>{ player_id: "Tiga", pos: 1, points: 562,5, money: 45, pay: 5},</v>
       </c>
       <c r="M298" t="str">
         <f t="shared" ref="M298:M305" si="50">CONCATENATE("{ player_id: """,G298,""", pos: ",H298,", points: ",I298,", money: ",J298,", pay: ",K298,"},")</f>
-        <v>{ player_id: "Tiga", pos: 1, points: 562.5, money: 50, pay: 5},</v>
+        <v>{ player_id: "Tiga", pos: 1, points: 562,5, money: 45, pay: 5},</v>
       </c>
     </row>
     <row r="299" spans="1:13" x14ac:dyDescent="0.25">
@@ -9255,8 +9258,8 @@
         <v>5</v>
       </c>
       <c r="L306" t="str">
-        <f>CONCATENATE("{ player_id: """,G306,""", pos: ",H306,", points: ",I306,", money: ",J306,", pay: ",K306,"}")</f>
-        <v>{ player_id: "Pipps", pos: 9, points: 62.5, money: 0, pay: 5}</v>
+        <f t="shared" si="49"/>
+        <v>{ player_id: "Pipps", pos: 9, points: 62,5, money: 0, pay: 5},</v>
       </c>
       <c r="M306" t="str">
         <f>CONCATENATE("{ player_id: """,G306,""", pos: ",H306,", points: ",I306,", money: ",J306,", pay: ",K306,"}")</f>
@@ -11588,7 +11591,7 @@
         <v>{ player_id: "Piretta", pos: 7, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="401" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C401" s="1"/>
       <c r="D401" s="1"/>
       <c r="G401" t="s">
@@ -11615,7 +11618,7 @@
         <v>{ player_id: "Suarez", pos: 8, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="402" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G402" t="s">
         <v>13</v>
       </c>
@@ -11640,7 +11643,7 @@
         <v>{ player_id: "Ben", pos: 9, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="403" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C403" s="1"/>
       <c r="D403" s="1"/>
       <c r="G403" t="s">
@@ -11667,7 +11670,7 @@
         <v>{ player_id: "Rico", pos: 10, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="404" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C404" s="1"/>
       <c r="D404" s="1"/>
       <c r="G404" t="s">
@@ -11694,7 +11697,7 @@
         <v>{ player_id: "Edo", pos: 11, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="405" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G405" t="s">
         <v>3</v>
       </c>
@@ -11719,7 +11722,7 @@
         <v>{ player_id: "Vale", pos: 12, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="406" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G406" t="s">
         <v>14</v>
       </c>
@@ -11744,7 +11747,7 @@
         <v>{ player_id: "Nero", pos: 13, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="407" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G407" t="s">
         <v>19</v>
       </c>
@@ -11769,7 +11772,7 @@
         <v>{ player_id: "Pipps", pos: 14, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="408" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G408" t="s">
         <v>20</v>
       </c>
@@ -11794,7 +11797,7 @@
         <v>{ player_id: "Riw", pos: 15, points: 0, money: 0, pay: 5},</v>
       </c>
     </row>
-    <row r="409" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L409" t="s">
         <v>108</v>
       </c>
@@ -11802,36 +11805,281 @@
         <v>109</v>
       </c>
     </row>
-    <row r="410" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H410" t="s">
+    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A410" s="4">
+        <v>136</v>
+      </c>
+      <c r="B410" s="5">
+        <v>2015</v>
+      </c>
+      <c r="C410" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E410" s="4">
+        <v>1</v>
+      </c>
+      <c r="F410" s="4">
+        <v>0</v>
+      </c>
+      <c r="L410" t="str">
+        <f>CONCATENATE("db.tournaments.insert({_id: ",A410,",year: ",B410,",date: ISODate(""",C410,"""),details: {location: """,D410,""",tables: ",E410,",final: ",F410,"},results: [")</f>
+        <v>db.tournaments.insert({_id: 136,year: 2015,date: ISODate("2015-01-02"),details: {location: "Cantina",tables: 1,final: 0},results: [</v>
+      </c>
+      <c r="M410" t="str">
+        <f>CONCATENATE("db.tournaments.update({_id: """,A410,"""},{$set: {year: ",B410,",date: ISODate(""",C410,"""),details: {location: """,D410,""",tables: ",E410,",final: ",F410,"},results: [")</f>
+        <v>db.tournaments.update({_id: "136"},{$set: {year: 2015,date: ISODate("2015-01-02"),details: {location: "Cantina",tables: 1,final: 0},results: [</v>
+      </c>
+    </row>
+    <row r="411" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G411" t="s">
+        <v>2</v>
+      </c>
+      <c r="H411">
+        <v>1</v>
+      </c>
+      <c r="I411">
+        <v>562.5</v>
+      </c>
+      <c r="J411">
+        <v>45</v>
+      </c>
+      <c r="K411">
+        <v>5</v>
+      </c>
+      <c r="L411" t="str">
+        <f>CONCATENATE("{ player_id: """,G411,""", pos: ",H411,", points: ",I411,", money: ",J411,", pay: ",K411,"},")</f>
+        <v>{ player_id: "Tiga", pos: 1, points: 562.5, money: 45, pay: 5},</v>
+      </c>
+      <c r="M411" t="str">
+        <f t="shared" ref="M411:M418" si="71">CONCATENATE("{ player_id: """,G411,""", pos: ",H411,", points: ",I411,", money: ",J411,", pay: ",K411,"},")</f>
+        <v>{ player_id: "Tiga", pos: 1, points: 562,5, money: 45, pay: 5},</v>
+      </c>
+    </row>
+    <row r="412" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C412" s="1"/>
+      <c r="D412" s="1"/>
+      <c r="G412" t="s">
+        <v>5</v>
+      </c>
+      <c r="H412">
+        <v>2</v>
+      </c>
+      <c r="I412">
+        <v>281.25</v>
+      </c>
+      <c r="J412">
+        <v>0</v>
+      </c>
+      <c r="K412">
+        <v>5</v>
+      </c>
+      <c r="L412" t="str">
+        <f>CONCATENATE("{ player_id: """,G412,""", pos: ",H412,", points: ",I412,", money: ",J412,", pay: ",K412,"},")</f>
+        <v>{ player_id: "Suarez", pos: 2, points: 281.25, money: 0, pay: 5},</v>
+      </c>
+      <c r="M412" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Suarez", pos: 2, points: 281,25, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C413" s="1"/>
+      <c r="D413" s="1"/>
+      <c r="G413" t="s">
+        <v>10</v>
+      </c>
+      <c r="H413">
+        <v>3</v>
+      </c>
+      <c r="I413">
+        <v>187.5</v>
+      </c>
+      <c r="J413">
+        <v>0</v>
+      </c>
+      <c r="K413">
+        <v>5</v>
+      </c>
+      <c r="L413" t="str">
+        <f>CONCATENATE("{ player_id: """,G413,""", pos: ",H413,", points: ",I413,", money: ",J413,", pay: ",K413,"},")</f>
+        <v>{ player_id: "Matteo", pos: 3, points: 187.5, money: 0, pay: 5},</v>
+      </c>
+      <c r="M413" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Matteo", pos: 3, points: 187,5, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C414" s="1"/>
+      <c r="D414" s="1"/>
+      <c r="G414" t="s">
         <v>12</v>
       </c>
-      <c r="I410">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="411" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H411" t="s">
-        <v>14</v>
-      </c>
-      <c r="I411">
-        <v>-0.01</v>
-      </c>
-    </row>
-    <row r="412" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H412" t="s">
+      <c r="H414">
+        <v>4</v>
+      </c>
+      <c r="I414">
+        <v>140.62</v>
+      </c>
+      <c r="J414">
+        <v>0</v>
+      </c>
+      <c r="K414">
+        <v>5</v>
+      </c>
+      <c r="L414" t="str">
+        <f>CONCATENATE("{ player_id: """,G414,""", pos: ",H414,", points: ",I414,", money: ",J414,", pay: ",K414,"},")</f>
+        <v>{ player_id: "Stecca", pos: 4, points: 140.62, money: 0, pay: 5},</v>
+      </c>
+      <c r="M414" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Stecca", pos: 4, points: 140,62, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C415" s="1"/>
+      <c r="D415" s="1"/>
+      <c r="G415" t="s">
+        <v>21</v>
+      </c>
+      <c r="H415">
+        <v>5</v>
+      </c>
+      <c r="I415">
+        <v>112.5</v>
+      </c>
+      <c r="J415">
+        <v>0</v>
+      </c>
+      <c r="K415">
+        <v>5</v>
+      </c>
+      <c r="L415" t="str">
+        <f>CONCATENATE("{ player_id: """,G415,""", pos: ",H415,", points: ",I415,", money: ",J415,", pay: ",K415,"},")</f>
+        <v>{ player_id: "Ciodo", pos: 5, points: 112.5, money: 0, pay: 5},</v>
+      </c>
+      <c r="M415" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Ciodo", pos: 5, points: 112,5, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C416" s="1"/>
+      <c r="D416" s="1"/>
+      <c r="G416" t="s">
+        <v>19</v>
+      </c>
+      <c r="H416">
+        <v>6</v>
+      </c>
+      <c r="I416">
+        <v>93.75</v>
+      </c>
+      <c r="J416">
+        <v>0</v>
+      </c>
+      <c r="K416">
+        <v>5</v>
+      </c>
+      <c r="L416" t="str">
+        <f>CONCATENATE("{ player_id: """,G416,""", pos: ",H416,", points: ",I416,", money: ",J416,", pay: ",K416,"},")</f>
+        <v>{ player_id: "Pipps", pos: 6, points: 93.75, money: 0, pay: 5},</v>
+      </c>
+      <c r="M416" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Pipps", pos: 6, points: 93,75, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="417" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C417" s="1"/>
+      <c r="D417" s="1"/>
+      <c r="G417" t="s">
         <v>9</v>
       </c>
-      <c r="I412">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="413" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H413" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I413">
-        <v>-0.3</v>
+      <c r="H417">
+        <v>7</v>
+      </c>
+      <c r="I417">
+        <v>80.31</v>
+      </c>
+      <c r="J417">
+        <v>0</v>
+      </c>
+      <c r="K417">
+        <v>5</v>
+      </c>
+      <c r="L417" t="str">
+        <f>CONCATENATE("{ player_id: """,G417,""", pos: ",H417,", points: ",I417,", money: ",J417,", pay: ",K417,"},")</f>
+        <v>{ player_id: "Busca", pos: 7, points: 80.31, money: 0, pay: 5},</v>
+      </c>
+      <c r="M417" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Busca", pos: 7, points: 80,31, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="418" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C418" s="1"/>
+      <c r="D418" s="1"/>
+      <c r="G418" t="s">
+        <v>6</v>
+      </c>
+      <c r="H418">
+        <v>8</v>
+      </c>
+      <c r="I418">
+        <v>70.31</v>
+      </c>
+      <c r="J418">
+        <v>0</v>
+      </c>
+      <c r="K418">
+        <v>5</v>
+      </c>
+      <c r="L418" t="str">
+        <f>CONCATENATE("{ player_id: """,G418,""", pos: ",H418,", points: ",I418,", money: ",J418,", pay: ",K418,"},")</f>
+        <v>{ player_id: "Rico", pos: 8, points: 70.31, money: 0, pay: 5},</v>
+      </c>
+      <c r="M418" t="str">
+        <f t="shared" si="71"/>
+        <v>{ player_id: "Rico", pos: 8, points: 70,31, money: 0, pay: 5},</v>
+      </c>
+    </row>
+    <row r="419" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C419" s="1"/>
+      <c r="D419" s="1"/>
+      <c r="G419" t="s">
+        <v>8</v>
+      </c>
+      <c r="H419">
+        <v>9</v>
+      </c>
+      <c r="I419">
+        <v>62.5</v>
+      </c>
+      <c r="J419">
+        <v>0</v>
+      </c>
+      <c r="K419">
+        <v>5</v>
+      </c>
+      <c r="L419" t="str">
+        <f>CONCATENATE("{ player_id: """,G419,""", pos: ",H419,", points: ",I419,", money: ",J419,", pay: ",K419,"},")</f>
+        <v>{ player_id: "Cana", pos: 9, points: 62.5, money: 0, pay: 5},</v>
+      </c>
+      <c r="M419" t="str">
+        <f>CONCATENATE("{ player_id: """,G419,""", pos: ",H419,", points: ",I419,", money: ",J419,", pay: ",K419,"}")</f>
+        <v>{ player_id: "Cana", pos: 9, points: 62,5, money: 0, pay: 5}</v>
+      </c>
+    </row>
+    <row r="420" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L420" t="s">
+        <v>108</v>
+      </c>
+      <c r="M420" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>